<commit_message>
SSDM-14128: Fixing failing test.
</commit_message>
<xml_diff>
--- a/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-vocabulary-property-compatible-with-import.xlsx
+++ b/openbis/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-vocabulary-property-compatible-with-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
   <si>
     <t xml:space="preserve">VOCABULARY_TYPE</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t xml:space="preserve">$BARCODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">Custom Barcode</t>
@@ -390,8 +393,8 @@
   </sheetPr>
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A18" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -537,9 +540,8 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C13" s="6" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C13" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>29</v>
@@ -562,21 +564,20 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C14" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C14" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,24 +588,23 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C15" s="6" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C15" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -639,17 +639,16 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="6" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,9 +691,8 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C21" s="6" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C21" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>29</v>
@@ -717,21 +715,20 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C22" s="6" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C22" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -742,24 +739,23 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="C23" s="6" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C23" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>29</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>